<commit_message>
Add script for generating embedding similarity features on proposed model
</commit_message>
<xml_diff>
--- a/summary/summary_week_50_100.xlsx
+++ b/summary/summary_week_50_100.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hankyu\Desktop\BAX\model_comparison\summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sulyunlee/Desktop/OHC/model_comparison/summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3673375-B7A3-43A8-BC4E-FE39F80E876D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE25A17-1BA0-0F47-BEF8-BA44EABAEE75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6618" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="19200" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary_week_50_100 - Copy" sheetId="1" r:id="rId1"/>
@@ -815,14 +815,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -1150,18 +1143,18 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>18</v>
       </c>
@@ -1184,7 +1177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
@@ -1211,7 +1204,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
       <c r="B3" s="13" t="s">
         <v>7</v>
@@ -1235,7 +1228,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -1259,7 +1252,7 @@
         <v>4.3630892943880499E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="16"/>
       <c r="B5" s="13" t="s">
         <v>9</v>
@@ -1283,7 +1276,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="13" t="s">
         <v>10</v>
@@ -1307,7 +1300,7 @@
         <v>4.6178460859155598E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="13" t="s">
         <v>11</v>
@@ -1331,7 +1324,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="13" t="s">
         <v>12</v>
@@ -1355,7 +1348,7 @@
         <v>4.9567988731444197E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="14" t="s">
         <v>13</v>
@@ -1379,7 +1372,7 @@
         <v>4.2159223641796296E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>16</v>
       </c>
@@ -1405,7 +1398,7 @@
         <v>0.11560750360750301</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="13" t="s">
         <v>7</v>
@@ -1429,7 +1422,7 @@
         <v>0.16800000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="13" t="s">
         <v>8</v>
@@ -1453,7 +1446,7 @@
         <v>0.155845922263322</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="13" t="s">
         <v>9</v>
@@ -1477,7 +1470,7 @@
         <v>0.159999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="13" t="s">
         <v>10</v>
@@ -1501,7 +1494,7 @@
         <v>0.15463839514032701</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="13" t="s">
         <v>11</v>
@@ -1525,7 +1518,7 @@
         <v>0.13120000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="13" t="s">
         <v>12</v>
@@ -1549,7 +1542,7 @@
         <v>0.136251261287372</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="14" t="s">
         <v>13</v>
@@ -1573,7 +1566,7 @@
         <v>4.9537566805579903E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>17</v>
       </c>
@@ -1599,7 +1592,7 @@
         <v>3.3018705844493401E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="13" t="s">
         <v>7</v>
@@ -1623,7 +1616,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="13" t="s">
         <v>8</v>
@@ -1647,7 +1640,7 @@
         <v>4.0186121156406303E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="13" t="s">
         <v>9</v>
@@ -1671,7 +1664,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
       <c r="B22" s="13" t="s">
         <v>10</v>
@@ -1695,7 +1688,7 @@
         <v>4.6026841671599601E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" s="13" t="s">
         <v>11</v>
@@ -1719,7 +1712,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" s="13" t="s">
         <v>12</v>
@@ -1743,7 +1736,7 @@
         <v>4.55786847491019E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="14" t="s">
         <v>13</v>
@@ -1767,7 +1760,7 @@
         <v>0.23215215490358701</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>14</v>
       </c>
@@ -1793,7 +1786,7 @@
         <v>0.101303018876548</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="13" t="s">
         <v>7</v>
@@ -1817,7 +1810,7 @@
         <v>0.183999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
       <c r="B28" s="13" t="s">
         <v>8</v>
@@ -1841,7 +1834,7 @@
         <v>0.19717187578661599</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
       <c r="B29" s="13" t="s">
         <v>9</v>
@@ -1865,7 +1858,7 @@
         <v>0.16899999999999901</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
       <c r="B30" s="13" t="s">
         <v>10</v>
@@ -1889,7 +1882,7 @@
         <v>0.18110812897384301</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="13" t="s">
         <v>11</v>
@@ -1913,7 +1906,7 @@
         <v>0.12759999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
       <c r="B32" s="13" t="s">
         <v>12</v>
@@ -1937,7 +1930,7 @@
         <v>0.14446224361183799</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="14" t="s">
         <v>13</v>
@@ -1969,10 +1962,10 @@
     <mergeCell ref="A26:A33"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:H33">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>C2=MAX($C2:$H2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>C2=MIN($C2:$H2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add new results to the summary file
</commit_message>
<xml_diff>
--- a/summary/summary_week_50_100.xlsx
+++ b/summary/summary_week_50_100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hankyu\Desktop\BAX\model_comparison\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6307ADA4-E66B-461F-BEA6-D503991B770A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A4DAC8-4C4A-4C6A-A4AC-8CA6D8C2A62E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="642" yWindow="462" windowWidth="19200" windowHeight="15762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
   <si>
     <t>baseline_agg</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>proposed_emb</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Neural
@@ -740,6 +737,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -754,9 +754,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1133,8 +1130,8 @@
   </sheetPr>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
@@ -1179,7 +1176,7 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1203,15 +1200,15 @@
       <c r="H2" s="1">
         <v>3.32637957005016E-2</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
+      <c r="I2" s="1">
+        <v>2.3474418466535401E-2</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.35729788102669E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="17"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
@@ -1233,15 +1230,15 @@
       <c r="H3" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>21</v>
+      <c r="I3" s="3">
+        <v>2.5999999999999902E-2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="17"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1263,15 +1260,15 @@
       <c r="H4" s="3">
         <v>4.3630892943880499E-2</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>21</v>
+      <c r="I4" s="3">
+        <v>2.1206918050881599E-2</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2.4360328290648402E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="17"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -1293,15 +1290,15 @@
       <c r="H5" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>21</v>
+      <c r="I5" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
@@ -1323,15 +1320,15 @@
       <c r="H6" s="3">
         <v>4.6178460859155598E-2</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>21</v>
+      <c r="I6" s="3">
+        <v>2.78223478109327E-2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>3.0538235616927301E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
@@ -1353,15 +1350,15 @@
       <c r="H7" s="3">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>21</v>
+      <c r="I7" s="3">
+        <v>4.24E-2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>3.9600000000000003E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
@@ -1383,15 +1380,15 @@
       <c r="H8" s="3">
         <v>4.9567988731444197E-2</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>21</v>
+      <c r="I8" s="3">
+        <v>3.7427105225206703E-2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>3.6182259395885201E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.7" thickBot="1">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="15" t="s">
         <v>13</v>
       </c>
@@ -1413,15 +1410,15 @@
       <c r="H9" s="5">
         <v>4.2159223641796296E-3</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>21</v>
+      <c r="I9" s="5">
+        <v>3.2745007642765601E-3</v>
+      </c>
+      <c r="J9" s="6">
+        <v>1.95748351218722E-3</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -1453,7 +1450,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
@@ -1483,7 +1480,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="17"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="12" t="s">
         <v>8</v>
       </c>
@@ -1513,7 +1510,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
@@ -1543,7 +1540,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="17"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="12" t="s">
         <v>10</v>
       </c>
@@ -1573,7 +1570,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="12" t="s">
         <v>11</v>
       </c>
@@ -1603,7 +1600,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="12" t="s">
         <v>12</v>
       </c>
@@ -1633,7 +1630,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.7" thickBot="1">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="15" t="s">
         <v>13</v>
       </c>
@@ -1663,7 +1660,7 @@
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
@@ -1687,15 +1684,15 @@
       <c r="H18" s="1">
         <v>3.3018705844493401E-2</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>21</v>
+      <c r="I18" s="1">
+        <v>3.8176090489465103E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>3.3100195304300702E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="17"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="12" t="s">
         <v>7</v>
       </c>
@@ -1717,15 +1714,15 @@
       <c r="H19" s="3">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>21</v>
+      <c r="I19" s="3">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.04</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="17"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="12" t="s">
         <v>8</v>
       </c>
@@ -1747,15 +1744,15 @@
       <c r="H20" s="3">
         <v>4.0186121156406303E-2</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>21</v>
+      <c r="I20" s="3">
+        <v>5.9126328631048601E-2</v>
+      </c>
+      <c r="J20" s="4">
+        <v>4.1727638833092599E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="17"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="12" t="s">
         <v>9</v>
       </c>
@@ -1777,15 +1774,15 @@
       <c r="H21" s="3">
         <v>4.7E-2</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>21</v>
+      <c r="I21" s="3">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J21" s="4">
+        <v>4.3999999999999997E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="17"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="12" t="s">
         <v>10</v>
       </c>
@@ -1807,15 +1804,15 @@
       <c r="H22" s="3">
         <v>4.6026841671599601E-2</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>21</v>
+      <c r="I22" s="3">
+        <v>5.7034538768146903E-2</v>
+      </c>
+      <c r="J22" s="4">
+        <v>4.3856603299669998E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="17"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="12" t="s">
         <v>11</v>
       </c>
@@ -1837,15 +1834,15 @@
       <c r="H23" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>21</v>
+      <c r="I23" s="3">
+        <v>5.3600000000000002E-2</v>
+      </c>
+      <c r="J23" s="4">
+        <v>4.1599999999999998E-2</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="17"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="12" t="s">
         <v>12</v>
       </c>
@@ -1867,15 +1864,15 @@
       <c r="H24" s="3">
         <v>4.55786847491019E-2</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>21</v>
+      <c r="I24" s="3">
+        <v>5.5119147840978301E-2</v>
+      </c>
+      <c r="J24" s="4">
+        <v>4.21365397678388E-2</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.7" thickBot="1">
-      <c r="A25" s="18"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="15" t="s">
         <v>13</v>
       </c>
@@ -1897,15 +1894,15 @@
       <c r="H25" s="5">
         <v>0.23215215490358701</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>21</v>
+      <c r="I25" s="5">
+        <v>0.30207188021173798</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0.30073465461485599</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -1937,7 +1934,7 @@
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="17"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="12" t="s">
         <v>7</v>
       </c>
@@ -1967,7 +1964,7 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="17"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1997,7 +1994,7 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="17"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="12" t="s">
         <v>9</v>
       </c>
@@ -2027,7 +2024,7 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="17"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="12" t="s">
         <v>10</v>
       </c>
@@ -2057,7 +2054,7 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="17"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="12" t="s">
         <v>11</v>
       </c>
@@ -2087,7 +2084,7 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="17"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="12" t="s">
         <v>12</v>
       </c>
@@ -2117,7 +2114,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="14.7" thickBot="1">
-      <c r="A33" s="18"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="15" t="s">
         <v>13</v>
       </c>
@@ -2147,8 +2144,8 @@
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="20" t="s">
-        <v>22</v>
+      <c r="A34" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>6</v>
@@ -2171,15 +2168,15 @@
       <c r="H34" s="3">
         <v>0.03</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>21</v>
+      <c r="I34" s="3">
+        <v>2.8571428571428501E-2</v>
+      </c>
+      <c r="J34" s="4">
+        <v>0.04</v>
       </c>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="17"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="12" t="s">
         <v>7</v>
       </c>
@@ -2201,15 +2198,15 @@
       <c r="H35" s="3">
         <v>0.17199999999999999</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>21</v>
+      <c r="I35" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.22399999999999901</v>
       </c>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="17"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="12" t="s">
         <v>8</v>
       </c>
@@ -2231,15 +2228,15 @@
       <c r="H36" s="3">
         <v>0.178382360972</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>21</v>
+      <c r="I36" s="3">
+        <v>0.164650083870541</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0.22893667156839301</v>
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="17"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="12" t="s">
         <v>9</v>
       </c>
@@ -2261,15 +2258,15 @@
       <c r="H37" s="3">
         <v>0.192</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>21</v>
+      <c r="I37" s="3">
+        <v>0.158</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0.184</v>
       </c>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="17"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="12" t="s">
         <v>10</v>
       </c>
@@ -2291,15 +2288,15 @@
       <c r="H38" s="3">
         <v>0.190787358543</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>21</v>
+      <c r="I38" s="3">
+        <v>0.162660913424754</v>
+      </c>
+      <c r="J38" s="4">
+        <v>0.19874511529818001</v>
       </c>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="17"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="12" t="s">
         <v>11</v>
       </c>
@@ -2321,15 +2318,15 @@
       <c r="H39" s="3">
         <v>0.1552</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>21</v>
+      <c r="I39" s="3">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="J39" s="4">
+        <v>0.1472</v>
       </c>
     </row>
     <row r="40" spans="1:10">
-      <c r="A40" s="17"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="12" t="s">
         <v>12</v>
       </c>
@@ -2351,15 +2348,15 @@
       <c r="H40" s="3">
         <v>0.16358513150099999</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>21</v>
+      <c r="I40" s="3">
+        <v>0.163641566110344</v>
+      </c>
+      <c r="J40" s="4">
+        <v>0.16448163504649199</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.7" thickBot="1">
-      <c r="A41" s="18"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="15" t="s">
         <v>13</v>
       </c>
@@ -2381,76 +2378,76 @@
       <c r="H41" s="5">
         <v>3.4710743801699999E-4</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>21</v>
+      <c r="I41" s="5">
+        <v>7.6523476523476504E-4</v>
+      </c>
+      <c r="J41" s="6">
+        <v>5.1804760895669897E-4</v>
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
     </row>
     <row r="49" spans="3:8">
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>